<commit_message>
fix label spacing; bump pkg version
</commit_message>
<xml_diff>
--- a/discussion/biplot-packages.xlsx
+++ b/discussion/biplot-packages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\R\projects\ggbiplot\discussion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648A6124-EEAE-4DA0-8888-6BE22487D1B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0FCE1D-373E-426C-B09D-C2F0C79AE2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="696" windowWidth="20064" windowHeight="11304" xr2:uid="{9C5127FA-2402-488A-ABC9-F429EC7F5995}"/>
+    <workbookView xWindow="2832" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{9C5127FA-2402-488A-ABC9-F429EC7F5995}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>package</t>
   </si>
@@ -123,6 +123,39 @@
   </si>
   <si>
     <t>The pcaMethods Package</t>
+  </si>
+  <si>
+    <t>Maintainer</t>
+  </si>
+  <si>
+    <t>friendly@yorku.ca</t>
+  </si>
+  <si>
+    <t>stephane.dray@univ-lyon1.fr</t>
+  </si>
+  <si>
+    <t>muvisu@sun.ac.za</t>
+  </si>
+  <si>
+    <t>francois.husson@institut-agro.fr</t>
+  </si>
+  <si>
+    <t>alboukadel.kassambara@gmail.com</t>
+  </si>
+  <si>
+    <t>ordr</t>
+  </si>
+  <si>
+    <t>villardon@usal.es</t>
+  </si>
+  <si>
+    <t>henning.red@gmail.com</t>
+  </si>
+  <si>
+    <t>cornelioid@gmail.com</t>
+  </si>
+  <si>
+    <t>Ordination in the tidyverse</t>
   </si>
 </sst>
 </file>
@@ -488,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55816383-A54F-4316-A729-FDE73AFBB1C2}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,9 +534,10 @@
     <col min="3" max="3" width="10.44140625" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="22.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +553,11 @@
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -537,7 +574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -547,8 +584,11 @@
       <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -559,7 +599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -569,8 +609,11 @@
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -578,7 +621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -588,8 +631,11 @@
       <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -599,8 +645,11 @@
       <c r="E9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -610,8 +659,11 @@
       <c r="E10" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -624,8 +676,11 @@
       <c r="E11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>26</v>
       </c>
@@ -634,6 +689,23 @@
       </c>
       <c r="E12" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -653,8 +725,14 @@
     <hyperlink ref="E3" r:id="rId13" xr:uid="{252378F2-869B-4080-91FD-A60BC7CF2988}"/>
     <hyperlink ref="A12" r:id="rId14" xr:uid="{3DBD22E2-59A8-4151-AFFD-D2547C5D5A4D}"/>
     <hyperlink ref="E12" r:id="rId15" xr:uid="{BE5C5EE6-50C3-4A99-91C2-580089CA5CEB}"/>
+    <hyperlink ref="F10" r:id="rId16" xr:uid="{6D54F244-3DE4-44B0-B139-B3F6A4BCF008}"/>
+    <hyperlink ref="F6" r:id="rId17" xr:uid="{81E6D87C-22D4-452D-8842-09917675E0AD}"/>
+    <hyperlink ref="F8" r:id="rId18" xr:uid="{53BDDFAA-8956-41AA-93FC-18383A989236}"/>
+    <hyperlink ref="F12" r:id="rId19" xr:uid="{E3554192-A3D6-4C22-97A5-083291D579CC}"/>
+    <hyperlink ref="A13" r:id="rId20" xr:uid="{0AE55237-CE65-4D93-A508-A2E8ED036250}"/>
+    <hyperlink ref="E13" r:id="rId21" xr:uid="{5B507CAA-F501-404B-B280-B8D886E55DA7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>